<commit_message>
Creado un modelo de regresión de aumento de gradiente
</commit_message>
<xml_diff>
--- a/predictions/Bosque Aleatorio de Regresión.xlsx
+++ b/predictions/Bosque Aleatorio de Regresión.xlsx
@@ -467,1313 +467,1313 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>450</v>
+        <v>139</v>
       </c>
       <c r="B2" t="n">
-        <v>2.897330164942685</v>
+        <v>20.9599858913756</v>
       </c>
       <c r="C2" t="n">
-        <v>2.878603320384749</v>
+        <v>20.90403992492036</v>
       </c>
       <c r="D2" t="n">
-        <v>5.052971911542515</v>
+        <v>32.51773770326</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>215</v>
+        <v>427</v>
       </c>
       <c r="B3" t="n">
-        <v>11.3512571527657</v>
+        <v>2.800759031013135</v>
       </c>
       <c r="C3" t="n">
-        <v>11.59185205628342</v>
+        <v>2.877806853067949</v>
       </c>
       <c r="D3" t="n">
-        <v>21.63641207734515</v>
+        <v>5.02767791353783</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>68</v>
+        <v>395</v>
       </c>
       <c r="B4" t="n">
-        <v>29.07085135648175</v>
+        <v>4.125897620764235</v>
       </c>
       <c r="C4" t="n">
-        <v>28.87077676386476</v>
+        <v>4.102873015732149</v>
       </c>
       <c r="D4" t="n">
-        <v>40.54943900848005</v>
+        <v>8.268354313217325</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>80</v>
+        <v>252</v>
       </c>
       <c r="B5" t="n">
-        <v>28.6337645865043</v>
+        <v>11.53340106378465</v>
       </c>
       <c r="C5" t="n">
-        <v>28.69767892765929</v>
+        <v>11.65912531797552</v>
       </c>
       <c r="D5" t="n">
-        <v>38.36414569134215</v>
+        <v>22.2917713397454</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="B6" t="n">
-        <v>29.07700898882855</v>
+        <v>20.97739451395675</v>
       </c>
       <c r="C6" t="n">
-        <v>28.84060829128769</v>
+        <v>20.76479150456611</v>
       </c>
       <c r="D6" t="n">
-        <v>39.83680291200081</v>
+        <v>30.52179847712515</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>294</v>
+        <v>127</v>
       </c>
       <c r="B7" t="n">
-        <v>6.68700480375266</v>
+        <v>27.44874821118845</v>
       </c>
       <c r="C7" t="n">
-        <v>6.548649961161022</v>
+        <v>27.01509082143413</v>
       </c>
       <c r="D7" t="n">
-        <v>12.8450840657745</v>
+        <v>37.00623732431945</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>36</v>
+        <v>317</v>
       </c>
       <c r="B8" t="n">
-        <v>27.47558094392985</v>
+        <v>6.496604118714695</v>
       </c>
       <c r="C8" t="n">
-        <v>26.65616204724239</v>
+        <v>6.545795983666207</v>
       </c>
       <c r="D8" t="n">
-        <v>44.52561048243</v>
+        <v>13.64131688836405</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="B9" t="n">
-        <v>27.80483933410755</v>
+        <v>20.73327055028665</v>
       </c>
       <c r="C9" t="n">
-        <v>28.33115874400587</v>
+        <v>20.81538630717223</v>
       </c>
       <c r="D9" t="n">
-        <v>39.00284580969505</v>
+        <v>32.13271098198495</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>349</v>
+        <v>171</v>
       </c>
       <c r="B10" t="n">
-        <v>4.054100319291375</v>
+        <v>19.6720855401965</v>
       </c>
       <c r="C10" t="n">
-        <v>4.082768314049888</v>
+        <v>20.88246733462378</v>
       </c>
       <c r="D10" t="n">
-        <v>7.639269730532945</v>
+        <v>31.1440779547959</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>313</v>
+        <v>451</v>
       </c>
       <c r="B11" t="n">
-        <v>6.791853483811765</v>
+        <v>2.87694343225705</v>
       </c>
       <c r="C11" t="n">
-        <v>6.498264069291745</v>
+        <v>2.891731732004348</v>
       </c>
       <c r="D11" t="n">
-        <v>13.38660917871345</v>
+        <v>5.228356319433136</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>177</v>
+        <v>225</v>
       </c>
       <c r="B12" t="n">
-        <v>21.5376937735259</v>
+        <v>11.5056173441023</v>
       </c>
       <c r="C12" t="n">
-        <v>20.76433304035237</v>
+        <v>11.59300916761727</v>
       </c>
       <c r="D12" t="n">
-        <v>32.995083577786</v>
+        <v>21.9023695482599</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>437</v>
+        <v>370</v>
       </c>
       <c r="B13" t="n">
-        <v>2.88576382711656</v>
+        <v>4.305819602350216</v>
       </c>
       <c r="C13" t="n">
-        <v>2.877558405977899</v>
+        <v>4.0868823277697</v>
       </c>
       <c r="D13" t="n">
-        <v>5.24585147124729</v>
+        <v>7.961658728183229</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>310</v>
+        <v>213</v>
       </c>
       <c r="B14" t="n">
-        <v>6.750367198202445</v>
+        <v>10.95876652639745</v>
       </c>
       <c r="C14" t="n">
-        <v>6.498305740941302</v>
+        <v>11.58694325653498</v>
       </c>
       <c r="D14" t="n">
-        <v>12.690801791674</v>
+        <v>22.92288929270335</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="B15" t="n">
-        <v>27.36924867030145</v>
+        <v>29.0031173422247</v>
       </c>
       <c r="C15" t="n">
-        <v>28.25781384089643</v>
+        <v>28.6598159713236</v>
       </c>
       <c r="D15" t="n">
-        <v>38.34450661918775</v>
+        <v>38.9002148804727</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G15" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>402</v>
+        <v>28</v>
       </c>
       <c r="B16" t="n">
-        <v>2.86774754682133</v>
+        <v>25.89256209928875</v>
       </c>
       <c r="C16" t="n">
-        <v>2.87604301019043</v>
+        <v>26.92951832553353</v>
       </c>
       <c r="D16" t="n">
-        <v>5.167424878856975</v>
+        <v>48.04703196347025</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G16" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>302</v>
+        <v>190</v>
       </c>
       <c r="B17" t="n">
-        <v>6.38323818293431</v>
+        <v>20.6905020299448</v>
       </c>
       <c r="C17" t="n">
-        <v>6.494698733845052</v>
+        <v>20.45633937098494</v>
       </c>
       <c r="D17" t="n">
-        <v>12.91264582031535</v>
+        <v>30.6275921054472</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G17" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>405</v>
+        <v>22</v>
       </c>
       <c r="B18" t="n">
-        <v>2.71732178197419</v>
+        <v>26.84187454938715</v>
       </c>
       <c r="C18" t="n">
-        <v>2.881790934405589</v>
+        <v>27.35977537769129</v>
       </c>
       <c r="D18" t="n">
-        <v>5.321456392902505</v>
+        <v>45.7670427074939</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>246</v>
+        <v>59</v>
       </c>
       <c r="B19" t="n">
-        <v>11.51900346563</v>
+        <v>27.44204718417045</v>
       </c>
       <c r="C19" t="n">
-        <v>11.59700593369628</v>
+        <v>26.34349931158438</v>
       </c>
       <c r="D19" t="n">
-        <v>22.4019032142076</v>
+        <v>43.2413534714904</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G19" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>329</v>
+        <v>215</v>
       </c>
       <c r="B20" t="n">
-        <v>6.59347113380073</v>
+        <v>11.3512571527657</v>
       </c>
       <c r="C20" t="n">
-        <v>6.6753054005634</v>
+        <v>11.59076504091947</v>
       </c>
       <c r="D20" t="n">
-        <v>12.89049503254035</v>
+        <v>21.63641207734515</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F20" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>350</v>
+        <v>14</v>
       </c>
       <c r="B21" t="n">
-        <v>4.127424222608395</v>
+        <v>29.01117004840865</v>
       </c>
       <c r="C21" t="n">
-        <v>4.082001203521266</v>
+        <v>27.73883463875579</v>
       </c>
       <c r="D21" t="n">
-        <v>8.30712335857511</v>
+        <v>47.52201565557725</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G21" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>260</v>
+        <v>10</v>
       </c>
       <c r="B22" t="n">
-        <v>12.05705788821515</v>
+        <v>29.403105022831</v>
       </c>
       <c r="C22" t="n">
-        <v>11.71771255250502</v>
+        <v>27.79713809523531</v>
       </c>
       <c r="D22" t="n">
-        <v>20.6809939223637</v>
+        <v>47.53285180572846</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F22" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>93</v>
+        <v>382</v>
       </c>
       <c r="B23" t="n">
-        <v>28.2680682394723</v>
+        <v>4.215885513358515</v>
       </c>
       <c r="C23" t="n">
-        <v>28.44737551877973</v>
+        <v>4.092040697654153</v>
       </c>
       <c r="D23" t="n">
-        <v>38.42296562349181</v>
+        <v>8.387584415584413</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G23" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>386</v>
+        <v>244</v>
       </c>
       <c r="B24" t="n">
-        <v>4.26109515382125</v>
+        <v>11.89535204006475</v>
       </c>
       <c r="C24" t="n">
-        <v>4.096253445981043</v>
+        <v>11.67525330784683</v>
       </c>
       <c r="D24" t="n">
-        <v>7.650961125312235</v>
+        <v>21.19252734003625</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>460</v>
+        <v>201</v>
       </c>
       <c r="B25" t="n">
-        <v>2.96592465753424</v>
+        <v>11.88448112336965</v>
       </c>
       <c r="C25" t="n">
-        <v>2.881200089768491</v>
+        <v>11.64682092702616</v>
       </c>
       <c r="D25" t="n">
-        <v>5.16949092587865</v>
+        <v>20.52815661706435</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>458</v>
+        <v>306</v>
       </c>
       <c r="B26" t="n">
-        <v>2.982861928046885</v>
+        <v>6.470909398635426</v>
       </c>
       <c r="C26" t="n">
-        <v>2.882444411656475</v>
+        <v>6.522062161785973</v>
       </c>
       <c r="D26" t="n">
-        <v>5.176794807430245</v>
+        <v>13.22150804309545</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F26" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G26" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>213</v>
+        <v>64</v>
       </c>
       <c r="B27" t="n">
-        <v>10.95876652639745</v>
+        <v>26.45301784973015</v>
       </c>
       <c r="C27" t="n">
-        <v>11.56183953825146</v>
+        <v>26.60317980079755</v>
       </c>
       <c r="D27" t="n">
-        <v>22.92288929270335</v>
+        <v>40.97289628180035</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F27" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="B28" t="n">
-        <v>28.46833859933215</v>
+        <v>20.6530483831049</v>
       </c>
       <c r="C28" t="n">
-        <v>28.33115874400587</v>
+        <v>20.87155533216857</v>
       </c>
       <c r="D28" t="n">
-        <v>37.28324738114415</v>
+        <v>31.5213182917002</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F28" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>435</v>
+        <v>339</v>
       </c>
       <c r="B29" t="n">
-        <v>2.728100703443165</v>
+        <v>3.89875532702995</v>
       </c>
       <c r="C29" t="n">
-        <v>2.870552282626177</v>
+        <v>4.080896768223652</v>
       </c>
       <c r="D29" t="n">
-        <v>5.4029880116645</v>
+        <v>8.301693916629841</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F29" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G29" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>238</v>
+        <v>290</v>
       </c>
       <c r="B30" t="n">
-        <v>12.29937921599195</v>
+        <v>6.432269068475815</v>
       </c>
       <c r="C30" t="n">
-        <v>11.61828328409191</v>
+        <v>6.529201404704429</v>
       </c>
       <c r="D30" t="n">
-        <v>22.0926038016353</v>
+        <v>13.13820623352755</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F30" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G30" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B31" t="n">
-        <v>4.104346461187211</v>
+        <v>4.26109515382125</v>
       </c>
       <c r="C31" t="n">
-        <v>4.101035813886853</v>
+        <v>4.086826964237111</v>
       </c>
       <c r="D31" t="n">
-        <v>7.758300891103895</v>
+        <v>7.650961125312235</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F31" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G31" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B32" t="n">
-        <v>29.3889612670434</v>
+        <v>26.6285488484118</v>
       </c>
       <c r="C32" t="n">
-        <v>28.83525267532246</v>
+        <v>26.91496611560198</v>
       </c>
       <c r="D32" t="n">
-        <v>39.34868851992135</v>
+        <v>44.88094422700585</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G32" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>278</v>
+        <v>351</v>
       </c>
       <c r="B33" t="n">
-        <v>6.369009863195664</v>
+        <v>4.128168980483645</v>
       </c>
       <c r="C33" t="n">
-        <v>6.526170546193222</v>
+        <v>4.083511751143453</v>
       </c>
       <c r="D33" t="n">
-        <v>14.39433555216485</v>
+        <v>8.260387497161885</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G33" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>316</v>
+        <v>273</v>
       </c>
       <c r="B34" t="n">
-        <v>6.644126779236045</v>
+        <v>6.382724960497701</v>
       </c>
       <c r="C34" t="n">
-        <v>6.517564087788373</v>
+        <v>6.529253911891931</v>
       </c>
       <c r="D34" t="n">
-        <v>14.38942658747915</v>
+        <v>13.5592785734052</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F34" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G34" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>236</v>
+        <v>342</v>
       </c>
       <c r="B35" t="n">
-        <v>11.54926657563195</v>
+        <v>4.057673950709085</v>
       </c>
       <c r="C35" t="n">
-        <v>11.57856978111419</v>
+        <v>4.067465699648414</v>
       </c>
       <c r="D35" t="n">
-        <v>20.72401491553</v>
+        <v>8.208044140030442</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G35" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="B36" t="n">
-        <v>20.36869003710445</v>
+        <v>11.3599108732552</v>
       </c>
       <c r="C36" t="n">
-        <v>20.60760638327485</v>
+        <v>11.65897126908586</v>
       </c>
       <c r="D36" t="n">
-        <v>31.17285964165035</v>
+        <v>23.0643850888043</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F36" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G36" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B37" t="n">
-        <v>6.470909398635426</v>
+        <v>6.955672217209409</v>
       </c>
       <c r="C37" t="n">
-        <v>6.503983391419805</v>
+        <v>6.525375848135768</v>
       </c>
       <c r="D37" t="n">
-        <v>13.22150804309545</v>
+        <v>13.3020198820895</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F37" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G37" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B38" t="n">
-        <v>26.50006631635425</v>
+        <v>20.7795861140381</v>
       </c>
       <c r="C38" t="n">
-        <v>27.3452902987748</v>
+        <v>20.83224716373105</v>
       </c>
       <c r="D38" t="n">
-        <v>37.7733700846295</v>
+        <v>31.7965777550906</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F38" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G38" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>255</v>
+        <v>110</v>
       </c>
       <c r="B39" t="n">
-        <v>11.5054965813739</v>
+        <v>28.10035196669485</v>
       </c>
       <c r="C39" t="n">
-        <v>11.65818246255115</v>
+        <v>28.08977144613683</v>
       </c>
       <c r="D39" t="n">
-        <v>20.4845419761183</v>
+        <v>37.92390957889926</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F39" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>301</v>
+        <v>33</v>
       </c>
       <c r="B40" t="n">
-        <v>6.482027859083125</v>
+        <v>24.77064579256355</v>
       </c>
       <c r="C40" t="n">
-        <v>6.492199126325698</v>
+        <v>27.14168060751892</v>
       </c>
       <c r="D40" t="n">
-        <v>12.0709314117598</v>
+        <v>45.92821917808215</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F40" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G40" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>433</v>
+        <v>87</v>
       </c>
       <c r="B41" t="n">
-        <v>2.81326447778502</v>
+        <v>28.11611720825225</v>
       </c>
       <c r="C41" t="n">
-        <v>2.868722994721939</v>
+        <v>28.67109607719678</v>
       </c>
       <c r="D41" t="n">
-        <v>5.139269699985695</v>
+        <v>38.16930439423585</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G41" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B42" t="n">
-        <v>28.02289628180035</v>
+        <v>27.76367755532135</v>
       </c>
       <c r="C42" t="n">
-        <v>28.28299640816238</v>
+        <v>28.31811518431077</v>
       </c>
       <c r="D42" t="n">
-        <v>46.96433463796475</v>
+        <v>44.7388166225394</v>
       </c>
       <c r="E42" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F42" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G42" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>206</v>
+        <v>434</v>
       </c>
       <c r="B43" t="n">
-        <v>11.83239178484755</v>
+        <v>2.712710584824675</v>
       </c>
       <c r="C43" t="n">
-        <v>11.56135043671648</v>
+        <v>2.87205249564114</v>
       </c>
       <c r="D43" t="n">
-        <v>21.64823232323225</v>
+        <v>5.217650671246555</v>
       </c>
       <c r="E43" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F43" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G43" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>171</v>
+        <v>91</v>
       </c>
       <c r="B44" t="n">
-        <v>19.6720855401965</v>
+        <v>27.7032903257572</v>
       </c>
       <c r="C44" t="n">
-        <v>20.91472677570573</v>
+        <v>28.47066168068413</v>
       </c>
       <c r="D44" t="n">
-        <v>31.1440779547959</v>
+        <v>38.10147801009365</v>
       </c>
       <c r="E44" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F44" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G44" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="B45" t="n">
-        <v>28.1752046124501</v>
+        <v>29.1204305283757</v>
       </c>
       <c r="C45" t="n">
-        <v>28.2287829523587</v>
+        <v>26.83116717920407</v>
       </c>
       <c r="D45" t="n">
-        <v>38.30890410958899</v>
+        <v>44.4960426179604</v>
       </c>
       <c r="E45" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F45" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G45" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>48</v>
+        <v>421</v>
       </c>
       <c r="B46" t="n">
-        <v>27.2432984152565</v>
+        <v>2.80724452878486</v>
       </c>
       <c r="C46" t="n">
-        <v>26.40201697265866</v>
+        <v>2.870637298265838</v>
       </c>
       <c r="D46" t="n">
-        <v>43.96776511160066</v>
+        <v>5.160992170249379</v>
       </c>
       <c r="E46" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F46" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G46" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>1</v>
+        <v>338</v>
       </c>
       <c r="B47" t="n">
-        <v>28.40184931506845</v>
+        <v>4.19652040143579</v>
       </c>
       <c r="C47" t="n">
-        <v>28.27235172485646</v>
+        <v>4.080896768223652</v>
       </c>
       <c r="D47" t="n">
-        <v>44.64306287319985</v>
+        <v>7.752918345420355</v>
       </c>
       <c r="E47" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F47" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G47" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>218</v>
+        <v>122</v>
       </c>
       <c r="B48" t="n">
-        <v>11.8359149334335</v>
+        <v>27.3548695368558</v>
       </c>
       <c r="C48" t="n">
-        <v>11.61358737332473</v>
+        <v>27.10943673198355</v>
       </c>
       <c r="D48" t="n">
-        <v>22.9230376307228</v>
+        <v>37.32402836521256</v>
       </c>
       <c r="E48" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F48" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G48" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>193</v>
+        <v>70</v>
       </c>
       <c r="B49" t="n">
-        <v>20.21633574234485</v>
+        <v>29.07700898882855</v>
       </c>
       <c r="C49" t="n">
-        <v>20.64689567588843</v>
+        <v>28.86728834923154</v>
       </c>
       <c r="D49" t="n">
-        <v>31.25784569188</v>
+        <v>39.83680291200081</v>
       </c>
       <c r="E49" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F49" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G49" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>229</v>
+        <v>378</v>
       </c>
       <c r="B50" t="n">
-        <v>11.5677803224149</v>
+        <v>4.07590274377979</v>
       </c>
       <c r="C50" t="n">
-        <v>11.635829115608</v>
+        <v>4.072854824710896</v>
       </c>
       <c r="D50" t="n">
-        <v>21.0488634171693</v>
+        <v>8.391615910640075</v>
       </c>
       <c r="E50" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F50" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G50" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="B51" t="n">
-        <v>28.545191858655</v>
+        <v>27.94282171025315</v>
       </c>
       <c r="C51" t="n">
-        <v>28.66051125101441</v>
+        <v>27.04905462524603</v>
       </c>
       <c r="D51" t="n">
-        <v>38.95817947190785</v>
+        <v>36.58958904109585</v>
       </c>
       <c r="E51" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F51" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G51" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="B52" t="n">
-        <v>2.905046882799155</v>
+        <v>3.016712407134565</v>
       </c>
       <c r="C52" t="n">
-        <v>2.872855396169589</v>
+        <v>2.88037466705758</v>
       </c>
       <c r="D52" t="n">
-        <v>5.086467627821484</v>
+        <v>5.079448863314489</v>
       </c>
       <c r="E52" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F52" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G52" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>319</v>
+        <v>137</v>
       </c>
       <c r="B53" t="n">
-        <v>6.595931220082495</v>
+        <v>20.66005377561415</v>
       </c>
       <c r="C53" t="n">
-        <v>6.577340581397715</v>
+        <v>20.79756347800249</v>
       </c>
       <c r="D53" t="n">
-        <v>12.7448319708632</v>
+        <v>31.62597394361085</v>
       </c>
       <c r="E53" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F53" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G53" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>456</v>
+        <v>288</v>
       </c>
       <c r="B54" t="n">
-        <v>2.77836622267112</v>
+        <v>6.58871580816344</v>
       </c>
       <c r="C54" t="n">
-        <v>2.874964202471261</v>
+        <v>6.543919428877943</v>
       </c>
       <c r="D54" t="n">
-        <v>5.079238179090231</v>
+        <v>12.25928710557065</v>
       </c>
       <c r="E54" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F54" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G54" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>202</v>
+        <v>408</v>
       </c>
       <c r="B55" t="n">
-        <v>11.630632439277</v>
+        <v>2.897372341971065</v>
       </c>
       <c r="C55" t="n">
-        <v>11.65125556785728</v>
+        <v>2.874156475623821</v>
       </c>
       <c r="D55" t="n">
-        <v>20.99751107002915</v>
+        <v>5.27378821482931</v>
       </c>
       <c r="E55" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F55" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G55" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B56" t="n">
-        <v>3.92322073349704</v>
+        <v>4.155383745283665</v>
       </c>
       <c r="C56" t="n">
-        <v>4.086468642072862</v>
+        <v>4.068622429196513</v>
       </c>
       <c r="D56" t="n">
-        <v>8.450179815833931</v>
+        <v>8.333400832356144</v>
       </c>
       <c r="E56" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F56" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G56" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>291</v>
+        <v>358</v>
       </c>
       <c r="B57" t="n">
-        <v>6.526828770999526</v>
+        <v>4.02115385783404</v>
       </c>
       <c r="C57" t="n">
-        <v>6.524552964834049</v>
+        <v>4.069589456129087</v>
       </c>
       <c r="D57" t="n">
-        <v>12.7870511252446</v>
+        <v>8.03734911678969</v>
       </c>
       <c r="E57" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F57" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G57" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>170</v>
+        <v>73</v>
       </c>
       <c r="B58" t="n">
-        <v>20.8837850889423</v>
+        <v>29.3889612670434</v>
       </c>
       <c r="C58" t="n">
-        <v>20.74170047925181</v>
+        <v>28.86666046247609</v>
       </c>
       <c r="D58" t="n">
-        <v>30.72564528171385</v>
+        <v>39.34868851992135</v>
       </c>
       <c r="E58" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F58" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G58" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="59">
@@ -1784,824 +1784,824 @@
         <v>29.0568582102828</v>
       </c>
       <c r="C59" t="n">
-        <v>28.44737551877973</v>
+        <v>28.47066168068413</v>
       </c>
       <c r="D59" t="n">
         <v>37.9410281499322</v>
       </c>
       <c r="E59" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F59" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G59" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>97</v>
+        <v>297</v>
       </c>
       <c r="B60" t="n">
-        <v>28.45770140247875</v>
+        <v>6.465400176089595</v>
       </c>
       <c r="C60" t="n">
-        <v>28.44260866100495</v>
+        <v>6.566588983586623</v>
       </c>
       <c r="D60" t="n">
-        <v>39.14278243860895</v>
+        <v>12.8205039608584</v>
       </c>
       <c r="E60" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F60" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G60" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="B61" t="n">
-        <v>3.9245132458537</v>
+        <v>2.92522004691059</v>
       </c>
       <c r="C61" t="n">
-        <v>4.083148314304022</v>
+        <v>2.889748631400794</v>
       </c>
       <c r="D61" t="n">
-        <v>7.929068435894125</v>
+        <v>5.443854953039085</v>
       </c>
       <c r="E61" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F61" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G61" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B62" t="n">
-        <v>21.1807080934418</v>
+        <v>21.03915687301935</v>
       </c>
       <c r="C62" t="n">
-        <v>20.95568255600195</v>
+        <v>20.75512700946376</v>
       </c>
       <c r="D62" t="n">
-        <v>30.9470802001206</v>
+        <v>30.5560589571628</v>
       </c>
       <c r="E62" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F62" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G62" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>393</v>
+        <v>272</v>
       </c>
       <c r="B63" t="n">
-        <v>4.342172746003895</v>
+        <v>6.862180260884215</v>
       </c>
       <c r="C63" t="n">
-        <v>4.102862283283128</v>
+        <v>6.533224124987302</v>
       </c>
       <c r="D63" t="n">
-        <v>8.27981703833138</v>
+        <v>12.9099064820215</v>
       </c>
       <c r="E63" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F63" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G63" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>114</v>
+        <v>221</v>
       </c>
       <c r="B64" t="n">
-        <v>26.6436399217221</v>
+        <v>11.7194453187071</v>
       </c>
       <c r="C64" t="n">
-        <v>28.2287829523587</v>
+        <v>11.62957269298312</v>
       </c>
       <c r="D64" t="n">
-        <v>38.5122055826432</v>
+        <v>21.93031800391385</v>
       </c>
       <c r="E64" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F64" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G64" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>216</v>
+        <v>331</v>
       </c>
       <c r="B65" t="n">
-        <v>12.0109065596291</v>
+        <v>4.24725226307778</v>
       </c>
       <c r="C65" t="n">
-        <v>11.60820742932004</v>
+        <v>4.064850716728615</v>
       </c>
       <c r="D65" t="n">
-        <v>23.1208451826644</v>
+        <v>7.94763029444182</v>
       </c>
       <c r="E65" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F65" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G65" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="B66" t="n">
-        <v>29.0031173422247</v>
+        <v>28.00781348788195</v>
       </c>
       <c r="C66" t="n">
-        <v>28.65798789122158</v>
+        <v>27.75752616581673</v>
       </c>
       <c r="D66" t="n">
-        <v>38.9002148804727</v>
+        <v>45.87929984779295</v>
       </c>
       <c r="E66" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F66" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G66" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>440</v>
+        <v>117</v>
       </c>
       <c r="B67" t="n">
-        <v>2.83271747222255</v>
+        <v>28.1752046124501</v>
       </c>
       <c r="C67" t="n">
-        <v>2.875290176949456</v>
+        <v>28.09909172174619</v>
       </c>
       <c r="D67" t="n">
-        <v>5.368238680433775</v>
+        <v>38.30890410958899</v>
       </c>
       <c r="E67" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F67" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G67" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>406</v>
+        <v>344</v>
       </c>
       <c r="B68" t="n">
-        <v>2.86385240431255</v>
+        <v>3.94658274545462</v>
       </c>
       <c r="C68" t="n">
-        <v>2.881790934405589</v>
+        <v>4.063889700262129</v>
       </c>
       <c r="D68" t="n">
-        <v>4.970559128539636</v>
+        <v>8.740335865943365</v>
       </c>
       <c r="E68" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F68" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G68" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>180</v>
+        <v>103</v>
       </c>
       <c r="B69" t="n">
-        <v>20.94323883263845</v>
+        <v>28.512337873525</v>
       </c>
       <c r="C69" t="n">
-        <v>20.63137775369341</v>
+        <v>28.28539373209883</v>
       </c>
       <c r="D69" t="n">
-        <v>32.36772807222755</v>
+        <v>37.34741026866305</v>
       </c>
       <c r="E69" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F69" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G69" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>226</v>
+        <v>34</v>
       </c>
       <c r="B70" t="n">
-        <v>11.5379537309982</v>
+        <v>25.95525114155245</v>
       </c>
       <c r="C70" t="n">
-        <v>11.59832893683764</v>
+        <v>27.14168060751892</v>
       </c>
       <c r="D70" t="n">
-        <v>21.3165128052412</v>
+        <v>44.64738114423845</v>
       </c>
       <c r="E70" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F70" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G70" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>17</v>
+        <v>363</v>
       </c>
       <c r="B71" t="n">
-        <v>25.36833896696905</v>
+        <v>4.026963588005455</v>
       </c>
       <c r="C71" t="n">
-        <v>27.29109033307111</v>
+        <v>4.07552601490908</v>
       </c>
       <c r="D71" t="n">
-        <v>45.91615568601866</v>
+        <v>7.737472884339605</v>
       </c>
       <c r="E71" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F71" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G71" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c r="B72" t="n">
-        <v>6.955672217209409</v>
+        <v>4.11684835920434</v>
       </c>
       <c r="C72" t="n">
-        <v>6.515813573223546</v>
+        <v>4.066292075322392</v>
       </c>
       <c r="D72" t="n">
-        <v>13.3020198820895</v>
+        <v>7.734880653874235</v>
       </c>
       <c r="E72" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F72" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G72" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>276</v>
+        <v>223</v>
       </c>
       <c r="B73" t="n">
-        <v>6.506418664980745</v>
+        <v>11.1467930260705</v>
       </c>
       <c r="C73" t="n">
-        <v>6.559574298425506</v>
+        <v>11.5987206896585</v>
       </c>
       <c r="D73" t="n">
-        <v>13.5022437411431</v>
+        <v>21.3463454979623</v>
       </c>
       <c r="E73" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F73" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G73" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>12</v>
+        <v>259</v>
       </c>
       <c r="B74" t="n">
-        <v>28.07009428927235</v>
+        <v>11.483157430469</v>
       </c>
       <c r="C74" t="n">
-        <v>27.76537129139907</v>
+        <v>11.5861555093446</v>
       </c>
       <c r="D74" t="n">
-        <v>44.52559360730589</v>
+        <v>22.200244992755</v>
       </c>
       <c r="E74" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F74" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G74" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>234</v>
+        <v>461</v>
       </c>
       <c r="B75" t="n">
-        <v>11.4247355422093</v>
+        <v>2.85074914383561</v>
       </c>
       <c r="C75" t="n">
-        <v>11.58579675903528</v>
+        <v>2.891475537327267</v>
       </c>
       <c r="D75" t="n">
-        <v>21.69983467792875</v>
+        <v>5.361368397674685</v>
       </c>
       <c r="E75" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F75" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G75" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>352</v>
+        <v>52</v>
       </c>
       <c r="B76" t="n">
-        <v>4.22716658690096</v>
+        <v>24.77788649706455</v>
       </c>
       <c r="C76" t="n">
-        <v>4.083047440068655</v>
+        <v>26.59186135798781</v>
       </c>
       <c r="D76" t="n">
-        <v>7.895614659313285</v>
+        <v>47.50684931506845</v>
       </c>
       <c r="E76" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F76" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G76" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>163</v>
+        <v>85</v>
       </c>
       <c r="B77" t="n">
-        <v>21.14441192070775</v>
+        <v>28.5112425260618</v>
       </c>
       <c r="C77" t="n">
-        <v>20.66541858686444</v>
+        <v>28.65573969957358</v>
       </c>
       <c r="D77" t="n">
-        <v>31.18762322913</v>
+        <v>38.8587763791188</v>
       </c>
       <c r="E77" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F77" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G77" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="B78" t="n">
-        <v>30.14870319634695</v>
+        <v>11.6451410367553</v>
       </c>
       <c r="C78" t="n">
-        <v>28.27235172485646</v>
+        <v>11.65842520993866</v>
       </c>
       <c r="D78" t="n">
-        <v>45.67858581788875</v>
+        <v>21.72440284332905</v>
       </c>
       <c r="E78" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F78" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G78" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>421</v>
+        <v>149</v>
       </c>
       <c r="B79" t="n">
-        <v>2.80724452878486</v>
+        <v>21.42351000217435</v>
       </c>
       <c r="C79" t="n">
-        <v>2.867163997785494</v>
+        <v>20.87590688470952</v>
       </c>
       <c r="D79" t="n">
-        <v>5.160992170249379</v>
+        <v>31.86542823666175</v>
       </c>
       <c r="E79" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F79" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G79" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>353</v>
+        <v>294</v>
       </c>
       <c r="B80" t="n">
-        <v>4.046439073370145</v>
+        <v>6.68700480375266</v>
       </c>
       <c r="C80" t="n">
-        <v>4.078265072162846</v>
+        <v>6.53387920440883</v>
       </c>
       <c r="D80" t="n">
-        <v>8.20925790237513</v>
+        <v>12.8450840657745</v>
       </c>
       <c r="E80" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F80" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G80" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>455</v>
+        <v>147</v>
       </c>
       <c r="B81" t="n">
-        <v>2.91581008925784</v>
+        <v>19.30625166842285</v>
       </c>
       <c r="C81" t="n">
-        <v>2.873622877649093</v>
+        <v>20.71858850928312</v>
       </c>
       <c r="D81" t="n">
-        <v>5.043440483988425</v>
+        <v>31.03494775320305</v>
       </c>
       <c r="E81" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F81" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G81" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>133</v>
+        <v>300</v>
       </c>
       <c r="B82" t="n">
-        <v>21.2003270671134</v>
+        <v>6.436364364360715</v>
       </c>
       <c r="C82" t="n">
-        <v>20.68539419546723</v>
+        <v>6.523126302351451</v>
       </c>
       <c r="D82" t="n">
-        <v>32.35289812419755</v>
+        <v>13.46057484737835</v>
       </c>
       <c r="E82" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F82" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G82" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>29</v>
+        <v>435</v>
       </c>
       <c r="B83" t="n">
-        <v>28.26596417281345</v>
+        <v>2.728100703443165</v>
       </c>
       <c r="C83" t="n">
-        <v>26.73447751417774</v>
+        <v>2.87253750437539</v>
       </c>
       <c r="D83" t="n">
-        <v>44.77930836286995</v>
+        <v>5.4029880116645</v>
       </c>
       <c r="E83" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F83" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G83" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="B84" t="n">
-        <v>6.585917044614526</v>
+        <v>6.490330850681495</v>
       </c>
       <c r="C84" t="n">
-        <v>6.491553843425086</v>
+        <v>6.609906963198312</v>
       </c>
       <c r="D84" t="n">
-        <v>14.15886805216515</v>
+        <v>12.8168685331242</v>
       </c>
       <c r="E84" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F84" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G84" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>337</v>
+        <v>268</v>
       </c>
       <c r="B85" t="n">
-        <v>4.039254631720381</v>
+        <v>6.57464282390954</v>
       </c>
       <c r="C85" t="n">
-        <v>4.085174767593106</v>
+        <v>6.529039284320408</v>
       </c>
       <c r="D85" t="n">
-        <v>8.12406385658301</v>
+        <v>11.98946943738485</v>
       </c>
       <c r="E85" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F85" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G85" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>438</v>
+        <v>228</v>
       </c>
       <c r="B86" t="n">
-        <v>2.80790133097496</v>
+        <v>11.97301488465865</v>
       </c>
       <c r="C86" t="n">
-        <v>2.876300206841336</v>
+        <v>11.67739340574112</v>
       </c>
       <c r="D86" t="n">
-        <v>5.216599058677015</v>
+        <v>22.04957188343785</v>
       </c>
       <c r="E86" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F86" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G86" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="B87" t="n">
-        <v>26.3674597452535</v>
+        <v>30.26601344495175</v>
       </c>
       <c r="C87" t="n">
-        <v>26.2680754649258</v>
+        <v>27.92841944585497</v>
       </c>
       <c r="D87" t="n">
-        <v>42.9513127853881</v>
+        <v>46.25428082191775</v>
       </c>
       <c r="E87" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F87" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G87" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>366</v>
+        <v>172</v>
       </c>
       <c r="B88" t="n">
-        <v>4.031438931670825</v>
+        <v>21.41645847753645</v>
       </c>
       <c r="C88" t="n">
-        <v>4.083134086526632</v>
+        <v>20.91658343282791</v>
       </c>
       <c r="D88" t="n">
-        <v>8.319611586153915</v>
+        <v>31.3411008061873</v>
       </c>
       <c r="E88" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F88" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G88" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>380</v>
+        <v>443</v>
       </c>
       <c r="B89" t="n">
-        <v>4.111667567892329</v>
+        <v>2.7844797555628</v>
       </c>
       <c r="C89" t="n">
-        <v>4.090521624746081</v>
+        <v>2.880259113766991</v>
       </c>
       <c r="D89" t="n">
-        <v>7.694030263755385</v>
+        <v>5.220930374371145</v>
       </c>
       <c r="E89" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F89" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G89" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>407</v>
+        <v>447</v>
       </c>
       <c r="B90" t="n">
-        <v>3.02015093130395</v>
+        <v>2.854509612571885</v>
       </c>
       <c r="C90" t="n">
-        <v>2.871633167035276</v>
+        <v>2.889795398164989</v>
       </c>
       <c r="D90" t="n">
-        <v>5.133235972113329</v>
+        <v>5.288012496995909</v>
       </c>
       <c r="E90" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F90" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G90" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>263</v>
+        <v>169</v>
       </c>
       <c r="B91" t="n">
-        <v>11.56924091753265</v>
+        <v>20.6969420229694</v>
       </c>
       <c r="C91" t="n">
-        <v>11.75314862543737</v>
+        <v>20.67139103122094</v>
       </c>
       <c r="D91" t="n">
-        <v>21.56426458293135</v>
+        <v>30.88526650407915</v>
       </c>
       <c r="E91" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F91" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G91" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>409</v>
+        <v>166</v>
       </c>
       <c r="B92" t="n">
-        <v>2.791014483164405</v>
+        <v>20.3919073626406</v>
       </c>
       <c r="C92" t="n">
-        <v>2.871819073645337</v>
+        <v>20.82231335706973</v>
       </c>
       <c r="D92" t="n">
-        <v>5.08167304658315</v>
+        <v>30.67288297694615</v>
       </c>
       <c r="E92" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F92" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G92" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>195</v>
+        <v>269</v>
       </c>
       <c r="B93" t="n">
-        <v>21.23198982366615</v>
+        <v>6.56125893473555</v>
       </c>
       <c r="C93" t="n">
-        <v>20.69386930886616</v>
+        <v>6.524495759542203</v>
       </c>
       <c r="D93" t="n">
-        <v>30.77285791028735</v>
+        <v>13.3511737889371</v>
       </c>
       <c r="E93" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F93" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G93" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="B94" t="n">
-        <v>2.939494701195685</v>
+        <v>2.77568478363735</v>
       </c>
       <c r="C94" t="n">
-        <v>2.877179742987685</v>
+        <v>2.868004853997231</v>
       </c>
       <c r="D94" t="n">
-        <v>5.388000175035735</v>
+        <v>5.689806074084585</v>
       </c>
       <c r="E94" t="n">
-        <v>0.9976802716495914</v>
+        <v>0.996558313678799</v>
       </c>
       <c r="F94" t="n">
-        <v>0.3478859713931323</v>
+        <v>0.512836828305422</v>
       </c>
       <c r="G94" t="n">
-        <v>0.5898185919358021</v>
+        <v>0.7161262656162124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creado gráfico de correlaciones
</commit_message>
<xml_diff>
--- a/predictions/Bosque Aleatorio de Regresión.xlsx
+++ b/predictions/Bosque Aleatorio de Regresión.xlsx
@@ -477,7 +477,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>418</v>
+        <v>189</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -485,30 +485,30 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.92572823027093</v>
+        <v>20.19028963448255</v>
       </c>
       <c r="D2" t="n">
-        <v>2.851075750894186</v>
+        <v>20.66776436333865</v>
       </c>
       <c r="E2" t="n">
-        <v>5.1764302527159</v>
+        <v>30.34404238821395</v>
       </c>
       <c r="F2" t="n">
-        <v>5.232356754075491</v>
+        <v>30.84583837012148</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H2" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>158</v>
+        <v>272</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -516,30 +516,30 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>19.4064377349113</v>
+        <v>6.862180260884215</v>
       </c>
       <c r="D3" t="n">
-        <v>20.75178039055626</v>
+        <v>6.554771122576877</v>
       </c>
       <c r="E3" t="n">
-        <v>31.27743145935055</v>
+        <v>12.9099064820215</v>
       </c>
       <c r="F3" t="n">
-        <v>31.2127906334384</v>
+        <v>13.15620308417847</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H3" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>208</v>
+        <v>57</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -547,30 +547,30 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>11.16235954466045</v>
+        <v>25.09969558599695</v>
       </c>
       <c r="D4" t="n">
-        <v>11.62879155250002</v>
+        <v>26.35603833499285</v>
       </c>
       <c r="E4" t="n">
-        <v>22.1574685116489</v>
+        <v>46.0489199157007</v>
       </c>
       <c r="F4" t="n">
-        <v>22.31853155164011</v>
+        <v>44.076585015264</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H4" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -578,30 +578,30 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>21.13327172996315</v>
+        <v>21.03915687301935</v>
       </c>
       <c r="D5" t="n">
-        <v>20.83863444355361</v>
+        <v>20.7742604218307</v>
       </c>
       <c r="E5" t="n">
-        <v>31.063280578091</v>
+        <v>30.5560589571628</v>
       </c>
       <c r="F5" t="n">
-        <v>31.17371110610444</v>
+        <v>31.31276396553866</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H5" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -609,30 +609,30 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6.653314184710554</v>
+        <v>11.35561806914545</v>
       </c>
       <c r="D6" t="n">
-        <v>6.532060659432431</v>
+        <v>11.7576511239304</v>
       </c>
       <c r="E6" t="n">
-        <v>13.76204359268505</v>
+        <v>22.42221936195635</v>
       </c>
       <c r="F6" t="n">
-        <v>13.15467461133223</v>
+        <v>22.31386497640542</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H6" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>124</v>
+        <v>325</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -640,30 +640,30 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>27.62122941116125</v>
+        <v>6.527285334288965</v>
       </c>
       <c r="D7" t="n">
-        <v>27.01042554451376</v>
+        <v>6.581200021304404</v>
       </c>
       <c r="E7" t="n">
-        <v>37.6422831050228</v>
+        <v>13.4407950913858</v>
       </c>
       <c r="F7" t="n">
-        <v>37.45486629717144</v>
+        <v>12.75334177084276</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H7" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>234</v>
+        <v>277</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -671,30 +671,30 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11.4247355422093</v>
+        <v>6.201595575097221</v>
       </c>
       <c r="D8" t="n">
-        <v>11.61163542364059</v>
+        <v>6.572870403885609</v>
       </c>
       <c r="E8" t="n">
-        <v>21.69983467792875</v>
+        <v>13.22521955692545</v>
       </c>
       <c r="F8" t="n">
-        <v>21.81150062716228</v>
+        <v>13.08255904486321</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H8" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>309</v>
+        <v>87</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -702,30 +702,30 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6.77558610239797</v>
+        <v>28.11611720825225</v>
       </c>
       <c r="D9" t="n">
-        <v>6.518149191004488</v>
+        <v>28.72381013055914</v>
       </c>
       <c r="E9" t="n">
-        <v>13.46924430095925</v>
+        <v>38.16930439423585</v>
       </c>
       <c r="F9" t="n">
-        <v>13.37819694501263</v>
+        <v>39.12385974206266</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H9" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>414</v>
+        <v>289</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -733,30 +733,30 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2.943104549648655</v>
+        <v>6.331452191759414</v>
       </c>
       <c r="D10" t="n">
-        <v>2.856863994832239</v>
+        <v>6.567125864972948</v>
       </c>
       <c r="E10" t="n">
-        <v>5.42059170444919</v>
+        <v>12.65626988853905</v>
       </c>
       <c r="F10" t="n">
-        <v>5.219373509514212</v>
+        <v>13.05824289700039</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H10" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>215</v>
+        <v>296</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -764,30 +764,30 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>11.3512571527657</v>
+        <v>6.39764700720502</v>
       </c>
       <c r="D11" t="n">
-        <v>11.52537184496263</v>
+        <v>6.555557781254863</v>
       </c>
       <c r="E11" t="n">
-        <v>21.63641207734515</v>
+        <v>12.5033766257305</v>
       </c>
       <c r="F11" t="n">
-        <v>21.8400388187199</v>
+        <v>13.17374703387603</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H11" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>77</v>
+        <v>392</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -795,30 +795,30 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>28.64035501734655</v>
+        <v>4.292643167167235</v>
       </c>
       <c r="D12" t="n">
-        <v>28.68492505045043</v>
+        <v>4.104165937021572</v>
       </c>
       <c r="E12" t="n">
-        <v>38.5015369194787</v>
+        <v>7.901587570297515</v>
       </c>
       <c r="F12" t="n">
-        <v>38.89260986465789</v>
+        <v>7.969445662585706</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H12" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>450</v>
+        <v>21</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -826,30 +826,30 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2.897330164942685</v>
+        <v>24.7632420091324</v>
       </c>
       <c r="D13" t="n">
-        <v>2.858620929315787</v>
+        <v>27.430429056158</v>
       </c>
       <c r="E13" t="n">
-        <v>5.052971911542515</v>
+        <v>45.84659158590065</v>
       </c>
       <c r="F13" t="n">
-        <v>5.238956795408282</v>
+        <v>45.69737220918481</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H13" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>221</v>
+        <v>369</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -857,30 +857,30 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>11.7194453187071</v>
+        <v>3.815643074581425</v>
       </c>
       <c r="D14" t="n">
-        <v>11.62275822402559</v>
+        <v>4.095046428317948</v>
       </c>
       <c r="E14" t="n">
-        <v>21.93031800391385</v>
+        <v>8.15466095890411</v>
       </c>
       <c r="F14" t="n">
-        <v>21.76434234813975</v>
+        <v>7.979499942835612</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H14" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I14" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>3</v>
+        <v>348</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -888,30 +888,30 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>27.76367755532135</v>
+        <v>4.265441948687744</v>
       </c>
       <c r="D15" t="n">
-        <v>28.38518354989971</v>
+        <v>4.090489802281239</v>
       </c>
       <c r="E15" t="n">
-        <v>44.7388166225394</v>
+        <v>8.281836013466641</v>
       </c>
       <c r="F15" t="n">
-        <v>46.43201556967451</v>
+        <v>7.98313167125948</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H15" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -919,30 +919,30 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>11.1467930260705</v>
+        <v>11.6416474522155</v>
       </c>
       <c r="D16" t="n">
-        <v>11.58225825651495</v>
+        <v>11.59122092987414</v>
       </c>
       <c r="E16" t="n">
-        <v>21.3463454979623</v>
+        <v>22.68798510111965</v>
       </c>
       <c r="F16" t="n">
-        <v>21.70338190209102</v>
+        <v>21.82005574792193</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H16" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I16" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>376</v>
+        <v>417</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -950,30 +950,30 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4.24574843921728</v>
+        <v>2.921702026624595</v>
       </c>
       <c r="D17" t="n">
-        <v>4.079119568968132</v>
+        <v>2.875944845341002</v>
       </c>
       <c r="E17" t="n">
-        <v>7.72170464774376</v>
+        <v>5.295294281301185</v>
       </c>
       <c r="F17" t="n">
-        <v>8.009304361808312</v>
+        <v>5.179266950012508</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H17" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>187</v>
+        <v>343</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -981,30 +981,30 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>20.75454178543875</v>
+        <v>3.885442784544505</v>
       </c>
       <c r="D18" t="n">
-        <v>20.55188226215747</v>
+        <v>4.091682555332814</v>
       </c>
       <c r="E18" t="n">
-        <v>30.46447850424885</v>
+        <v>7.806880151811654</v>
       </c>
       <c r="F18" t="n">
-        <v>30.99936391521621</v>
+        <v>7.96906398582204</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H18" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I18" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>18</v>
+        <v>411</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1012,30 +1012,30 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>24.3946183953033</v>
+        <v>2.72731162505596</v>
       </c>
       <c r="D19" t="n">
-        <v>27.67256563316676</v>
+        <v>2.876849027634346</v>
       </c>
       <c r="E19" t="n">
-        <v>45.7850534615275</v>
+        <v>5.393070730956005</v>
       </c>
       <c r="F19" t="n">
-        <v>46.07866035142015</v>
+        <v>5.210541453765661</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H19" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I19" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>106</v>
+        <v>233</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1043,30 +1043,30 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>27.80483933410755</v>
+        <v>11.8891884420492</v>
       </c>
       <c r="D20" t="n">
-        <v>28.2378452454708</v>
+        <v>11.57298888640708</v>
       </c>
       <c r="E20" t="n">
-        <v>39.00284580969505</v>
+        <v>22.75069300882695</v>
       </c>
       <c r="F20" t="n">
-        <v>38.31372470754414</v>
+        <v>21.58626779157797</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H20" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I20" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1074,30 +1074,30 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.89899469235607</v>
+        <v>2.97324534010631</v>
       </c>
       <c r="D21" t="n">
-        <v>2.853472304604813</v>
+        <v>2.87552527099213</v>
       </c>
       <c r="E21" t="n">
-        <v>5.18490884746111</v>
+        <v>5.25764545708849</v>
       </c>
       <c r="F21" t="n">
-        <v>5.22258433477072</v>
+        <v>5.223412530668647</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H21" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I21" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>444</v>
+        <v>123</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1105,30 +1105,30 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.87852610949245</v>
+        <v>26.80513075965125</v>
       </c>
       <c r="D22" t="n">
-        <v>2.849899320936522</v>
+        <v>27.42976482309763</v>
       </c>
       <c r="E22" t="n">
-        <v>5.312480123161755</v>
+        <v>37.10972491066104</v>
       </c>
       <c r="F22" t="n">
-        <v>5.227284147005549</v>
+        <v>37.27087117449805</v>
       </c>
       <c r="G22" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H22" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I22" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>253</v>
+        <v>154</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1136,30 +1136,30 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>11.71642455717795</v>
+        <v>20.88558337703505</v>
       </c>
       <c r="D23" t="n">
-        <v>11.54260741004975</v>
+        <v>20.77676711151824</v>
       </c>
       <c r="E23" t="n">
-        <v>20.1999647645366</v>
+        <v>30.6067392859107</v>
       </c>
       <c r="F23" t="n">
-        <v>21.07348146017733</v>
+        <v>31.17962714675403</v>
       </c>
       <c r="G23" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H23" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I23" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1167,30 +1167,30 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>12.1166873393228</v>
+        <v>11.80330329945915</v>
       </c>
       <c r="D24" t="n">
-        <v>11.57231623910501</v>
+        <v>11.71725998278675</v>
       </c>
       <c r="E24" t="n">
-        <v>21.9492613771557</v>
+        <v>22.38732191273085</v>
       </c>
       <c r="F24" t="n">
-        <v>21.34758235845198</v>
+        <v>21.98837656048413</v>
       </c>
       <c r="G24" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H24" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I24" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>456</v>
+        <v>139</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1198,30 +1198,30 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2.77836622267112</v>
+        <v>20.9599858913756</v>
       </c>
       <c r="D25" t="n">
-        <v>2.851845449698637</v>
+        <v>20.88411738279961</v>
       </c>
       <c r="E25" t="n">
-        <v>5.079238179090231</v>
+        <v>32.51773770326</v>
       </c>
       <c r="F25" t="n">
-        <v>5.219960878770662</v>
+        <v>31.5259298126089</v>
       </c>
       <c r="G25" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H25" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I25" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1229,30 +1229,30 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>21.41645847753645</v>
+        <v>25.22103718199605</v>
       </c>
       <c r="D26" t="n">
-        <v>20.82753223216785</v>
+        <v>26.65125520030762</v>
       </c>
       <c r="E26" t="n">
-        <v>31.3411008061873</v>
+        <v>43.833293627159</v>
       </c>
       <c r="F26" t="n">
-        <v>31.16635399758303</v>
+        <v>44.55549563940158</v>
       </c>
       <c r="G26" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H26" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I26" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>237</v>
+        <v>350</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1260,30 +1260,30 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>11.0104675684178</v>
+        <v>4.127424222608395</v>
       </c>
       <c r="D27" t="n">
-        <v>11.63995173451</v>
+        <v>4.090265745258013</v>
       </c>
       <c r="E27" t="n">
-        <v>22.395688214902</v>
+        <v>8.30712335857511</v>
       </c>
       <c r="F27" t="n">
-        <v>21.62530616981959</v>
+        <v>8.002080557613052</v>
       </c>
       <c r="G27" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H27" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I27" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>216</v>
+        <v>428</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1291,30 +1291,30 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.0109065596291</v>
+        <v>2.856330261365885</v>
       </c>
       <c r="D28" t="n">
-        <v>11.60220466376344</v>
+        <v>2.875456413892885</v>
       </c>
       <c r="E28" t="n">
-        <v>23.1208451826644</v>
+        <v>5.239716414323475</v>
       </c>
       <c r="F28" t="n">
-        <v>22.01699454373612</v>
+        <v>5.191253887963984</v>
       </c>
       <c r="G28" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H28" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I28" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>323</v>
+        <v>443</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1322,30 +1322,30 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6.73764337219117</v>
+        <v>2.7844797555628</v>
       </c>
       <c r="D29" t="n">
-        <v>6.521410503638285</v>
+        <v>2.874040614315783</v>
       </c>
       <c r="E29" t="n">
-        <v>13.0827432320943</v>
+        <v>5.220930374371145</v>
       </c>
       <c r="F29" t="n">
-        <v>12.78868401915078</v>
+        <v>5.229330857715097</v>
       </c>
       <c r="G29" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H29" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I29" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1353,30 +1353,30 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>12.05705788821515</v>
+        <v>11.5379537309982</v>
       </c>
       <c r="D30" t="n">
-        <v>11.75100972840969</v>
+        <v>11.57604339386582</v>
       </c>
       <c r="E30" t="n">
-        <v>20.6809939223637</v>
+        <v>21.3165128052412</v>
       </c>
       <c r="F30" t="n">
-        <v>21.80347086776496</v>
+        <v>21.77404451156247</v>
       </c>
       <c r="G30" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H30" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I30" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>122</v>
+        <v>248</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1384,30 +1384,30 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>27.3548695368558</v>
+        <v>11.8527227875338</v>
       </c>
       <c r="D31" t="n">
-        <v>27.01903256070733</v>
+        <v>11.60790682043174</v>
       </c>
       <c r="E31" t="n">
-        <v>37.32402836521256</v>
+        <v>21.4320405621775</v>
       </c>
       <c r="F31" t="n">
-        <v>37.53260006542793</v>
+        <v>22.15847978394176</v>
       </c>
       <c r="G31" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H31" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I31" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>31</v>
+        <v>447</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1415,30 +1415,30 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>25.16535907015355</v>
+        <v>2.854509612571885</v>
       </c>
       <c r="D32" t="n">
-        <v>27.53909547657663</v>
+        <v>2.880243500243389</v>
       </c>
       <c r="E32" t="n">
-        <v>45.15492882084335</v>
+        <v>5.288012496995909</v>
       </c>
       <c r="F32" t="n">
-        <v>45.33701809200782</v>
+        <v>5.229013971036982</v>
       </c>
       <c r="G32" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H32" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>218</v>
+        <v>69</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1446,30 +1446,30 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>11.8359149334335</v>
+        <v>29.96789330383725</v>
       </c>
       <c r="D33" t="n">
-        <v>11.62829968136449</v>
+        <v>28.84287032727883</v>
       </c>
       <c r="E33" t="n">
-        <v>22.9230376307228</v>
+        <v>38.7632952815829</v>
       </c>
       <c r="F33" t="n">
-        <v>22.12523855548895</v>
+        <v>39.60735212790932</v>
       </c>
       <c r="G33" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H33" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I33" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>246</v>
+        <v>460</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1477,30 +1477,30 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>11.51900346563</v>
+        <v>2.96592465753424</v>
       </c>
       <c r="D34" t="n">
-        <v>11.62701952895664</v>
+        <v>2.877868418154907</v>
       </c>
       <c r="E34" t="n">
-        <v>22.4019032142076</v>
+        <v>5.16949092587865</v>
       </c>
       <c r="F34" t="n">
-        <v>21.90334115422591</v>
+        <v>5.213912278387941</v>
       </c>
       <c r="G34" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H34" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I34" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>334</v>
+        <v>413</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1508,30 +1508,30 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>4.07709885315162</v>
+        <v>2.83072635987014</v>
       </c>
       <c r="D35" t="n">
-        <v>4.075675973737101</v>
+        <v>2.877421678129964</v>
       </c>
       <c r="E35" t="n">
-        <v>7.13663741568231</v>
+        <v>5.10808042048976</v>
       </c>
       <c r="F35" t="n">
-        <v>7.979933983288991</v>
+        <v>5.210325088698991</v>
       </c>
       <c r="G35" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H35" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I35" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1539,30 +1539,30 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>26.82276908023475</v>
+        <v>12.3617202404393</v>
       </c>
       <c r="D36" t="n">
-        <v>27.11547800590642</v>
+        <v>11.61168634445466</v>
       </c>
       <c r="E36" t="n">
-        <v>36.39545720161365</v>
+        <v>20.5201297104721</v>
       </c>
       <c r="F36" t="n">
-        <v>37.53893404354144</v>
+        <v>21.64922766441973</v>
       </c>
       <c r="G36" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H36" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I36" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>355</v>
+        <v>381</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1570,30 +1570,30 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3.96170938594873</v>
+        <v>4.055586645511115</v>
       </c>
       <c r="D37" t="n">
-        <v>4.073368959125307</v>
+        <v>4.096631012349644</v>
       </c>
       <c r="E37" t="n">
-        <v>7.833063172243235</v>
+        <v>8.21494227599484</v>
       </c>
       <c r="F37" t="n">
-        <v>7.997617177070913</v>
+        <v>7.991753428316931</v>
       </c>
       <c r="G37" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H37" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I37" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>441</v>
+        <v>223</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1601,30 +1601,30 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.97324534010631</v>
+        <v>11.1467930260705</v>
       </c>
       <c r="D38" t="n">
-        <v>2.84884592391571</v>
+        <v>11.56807796501738</v>
       </c>
       <c r="E38" t="n">
-        <v>5.25764545708849</v>
+        <v>21.3463454979623</v>
       </c>
       <c r="F38" t="n">
-        <v>5.246911005706501</v>
+        <v>21.6244066853989</v>
       </c>
       <c r="G38" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H38" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I38" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1632,30 +1632,30 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>29.3889612670434</v>
+        <v>20.84331728989255</v>
       </c>
       <c r="D39" t="n">
-        <v>28.93920928628154</v>
+        <v>20.86407393265565</v>
       </c>
       <c r="E39" t="n">
-        <v>39.34868851992135</v>
+        <v>31.9777070540072</v>
       </c>
       <c r="F39" t="n">
-        <v>39.69016703268814</v>
+        <v>31.49950681590811</v>
       </c>
       <c r="G39" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H39" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I39" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>103</v>
+        <v>368</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1663,30 +1663,30 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>28.512337873525</v>
+        <v>3.9245132458537</v>
       </c>
       <c r="D40" t="n">
-        <v>28.22522862693562</v>
+        <v>4.094295058856525</v>
       </c>
       <c r="E40" t="n">
-        <v>37.34741026866305</v>
+        <v>7.929068435894125</v>
       </c>
       <c r="F40" t="n">
-        <v>38.31288218717437</v>
+        <v>7.980989371968883</v>
       </c>
       <c r="G40" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H40" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I40" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1694,30 +1694,30 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>28.46833859933215</v>
+        <v>12.07045581808565</v>
       </c>
       <c r="D41" t="n">
-        <v>28.22719987100901</v>
+        <v>11.74861388258988</v>
       </c>
       <c r="E41" t="n">
-        <v>37.28324738114415</v>
+        <v>21.4354386800335</v>
       </c>
       <c r="F41" t="n">
-        <v>38.31719712022553</v>
+        <v>22.08190144011376</v>
       </c>
       <c r="G41" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H41" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I41" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>286</v>
+        <v>158</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1725,30 +1725,30 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6.74344913856463</v>
+        <v>19.4064377349113</v>
       </c>
       <c r="D42" t="n">
-        <v>6.549797804178513</v>
+        <v>20.65583686404225</v>
       </c>
       <c r="E42" t="n">
-        <v>12.9757855429146</v>
+        <v>31.27743145935055</v>
       </c>
       <c r="F42" t="n">
-        <v>13.08032278122555</v>
+        <v>31.26714663423561</v>
       </c>
       <c r="G42" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H42" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I42" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1756,30 +1756,30 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>27.4380136986301</v>
+        <v>25.83961239204635</v>
       </c>
       <c r="D43" t="n">
-        <v>27.23481328403149</v>
+        <v>27.42029254786935</v>
       </c>
       <c r="E43" t="n">
-        <v>44.4071232876712</v>
+        <v>36.4245931921959</v>
       </c>
       <c r="F43" t="n">
-        <v>45.66554797042554</v>
+        <v>37.2766926771639</v>
       </c>
       <c r="G43" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H43" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I43" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>391</v>
+        <v>420</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1787,30 +1787,30 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4.065584762845035</v>
+        <v>2.88218468308609</v>
       </c>
       <c r="D44" t="n">
-        <v>4.113435680543749</v>
+        <v>2.875469009496398</v>
       </c>
       <c r="E44" t="n">
-        <v>8.07358446793998</v>
+        <v>5.114012264960961</v>
       </c>
       <c r="F44" t="n">
-        <v>7.927915962443902</v>
+        <v>5.223828985585494</v>
       </c>
       <c r="G44" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H44" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I44" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>311</v>
+        <v>184</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1818,30 +1818,30 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>6.437393355628251</v>
+        <v>21.6586170692396</v>
       </c>
       <c r="D45" t="n">
-        <v>6.51511241189603</v>
+        <v>20.89080367907122</v>
       </c>
       <c r="E45" t="n">
-        <v>13.7517134489645</v>
+        <v>31.28971318769865</v>
       </c>
       <c r="F45" t="n">
-        <v>13.35309148055139</v>
+        <v>31.09851478196638</v>
       </c>
       <c r="G45" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H45" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I45" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>143</v>
+        <v>405</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1849,30 +1849,30 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>20.97739451395675</v>
+        <v>2.71732178197419</v>
       </c>
       <c r="D46" t="n">
-        <v>20.67274616831698</v>
+        <v>2.887012193592425</v>
       </c>
       <c r="E46" t="n">
-        <v>30.52179847712515</v>
+        <v>5.321456392902505</v>
       </c>
       <c r="F46" t="n">
-        <v>31.70206994267426</v>
+        <v>5.12759322042494</v>
       </c>
       <c r="G46" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H46" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I46" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1880,30 +1880,30 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>6.86551678796807</v>
+        <v>4.064965734589875</v>
       </c>
       <c r="D47" t="n">
-        <v>6.621609875611998</v>
+        <v>4.090547337582819</v>
       </c>
       <c r="E47" t="n">
-        <v>13.0945962186017</v>
+        <v>7.837295311779715</v>
       </c>
       <c r="F47" t="n">
-        <v>12.93724563447818</v>
+        <v>7.966047895921146</v>
       </c>
       <c r="G47" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H47" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I47" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>183</v>
+        <v>434</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1911,30 +1911,30 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>20.50486564243355</v>
+        <v>2.712710584824675</v>
       </c>
       <c r="D48" t="n">
-        <v>20.87334695068174</v>
+        <v>2.876701953037638</v>
       </c>
       <c r="E48" t="n">
-        <v>30.93111418799845</v>
+        <v>5.217650671246555</v>
       </c>
       <c r="F48" t="n">
-        <v>31.15037860780308</v>
+        <v>5.221419111794078</v>
       </c>
       <c r="G48" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H48" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I48" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1942,30 +1942,30 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.0362499617054</v>
+        <v>2.86774754682133</v>
       </c>
       <c r="D49" t="n">
-        <v>2.847180252369596</v>
+        <v>2.886693006264504</v>
       </c>
       <c r="E49" t="n">
-        <v>5.09712131535537</v>
+        <v>5.167424878856975</v>
       </c>
       <c r="F49" t="n">
-        <v>5.20217198243903</v>
+        <v>5.129513965574031</v>
       </c>
       <c r="G49" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H49" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I49" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>288</v>
+        <v>401</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1973,30 +1973,30 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6.58871580816344</v>
+        <v>2.830892476689645</v>
       </c>
       <c r="D50" t="n">
-        <v>6.524949738465132</v>
+        <v>2.886630683989267</v>
       </c>
       <c r="E50" t="n">
-        <v>12.25928710557065</v>
+        <v>5.430911292680635</v>
       </c>
       <c r="F50" t="n">
-        <v>13.12598033091237</v>
+        <v>5.12742859089276</v>
       </c>
       <c r="G50" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H50" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I50" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>294</v>
+        <v>6</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -2004,30 +2004,30 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6.68700480375266</v>
+        <v>24.9181430745814</v>
       </c>
       <c r="D51" t="n">
-        <v>6.535997519108884</v>
+        <v>28.47182735388139</v>
       </c>
       <c r="E51" t="n">
-        <v>12.8450840657745</v>
+        <v>46.45340675082815</v>
       </c>
       <c r="F51" t="n">
-        <v>13.11106036964325</v>
+        <v>46.17349071315217</v>
       </c>
       <c r="G51" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H51" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I51" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -2035,25 +2035,25 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>6.955672217209409</v>
+        <v>6.437393355628251</v>
       </c>
       <c r="D52" t="n">
-        <v>6.509092249070904</v>
+        <v>6.563387555306462</v>
       </c>
       <c r="E52" t="n">
-        <v>13.3020198820895</v>
+        <v>13.7517134489645</v>
       </c>
       <c r="F52" t="n">
-        <v>13.37203262218954</v>
+        <v>13.3197906486155</v>
       </c>
       <c r="G52" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H52" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I52" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="53">
@@ -2069,27 +2069,27 @@
         <v>25.43148769039175</v>
       </c>
       <c r="D53" t="n">
-        <v>26.2748173995521</v>
+        <v>26.63021598097716</v>
       </c>
       <c r="E53" t="n">
         <v>44.12783757338545</v>
       </c>
       <c r="F53" t="n">
-        <v>44.60408686875868</v>
+        <v>44.57375745530563</v>
       </c>
       <c r="G53" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H53" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I53" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>188</v>
+        <v>323</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -2097,30 +2097,30 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>20.36869003710445</v>
+        <v>6.73764337219117</v>
       </c>
       <c r="D54" t="n">
-        <v>20.64522569465958</v>
+        <v>6.546416919563489</v>
       </c>
       <c r="E54" t="n">
-        <v>31.17285964165035</v>
+        <v>13.0827432320943</v>
       </c>
       <c r="F54" t="n">
-        <v>31.11218454315544</v>
+        <v>12.71603963077078</v>
       </c>
       <c r="G54" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H54" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I54" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2128,30 +2128,30 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>29.0568582102828</v>
+        <v>27.2432984152565</v>
       </c>
       <c r="D55" t="n">
-        <v>28.54106951308638</v>
+        <v>26.65445394729171</v>
       </c>
       <c r="E55" t="n">
-        <v>37.9410281499322</v>
+        <v>43.96776511160066</v>
       </c>
       <c r="F55" t="n">
-        <v>38.71614496783313</v>
+        <v>44.54640543807582</v>
       </c>
       <c r="G55" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H55" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I55" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>458</v>
+        <v>398</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2159,30 +2159,30 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.982861928046885</v>
+        <v>2.90756924541539</v>
       </c>
       <c r="D56" t="n">
-        <v>2.857936250395719</v>
+        <v>2.885228769079055</v>
       </c>
       <c r="E56" t="n">
-        <v>5.176794807430245</v>
+        <v>5.28704924102184</v>
       </c>
       <c r="F56" t="n">
-        <v>5.228408285428426</v>
+        <v>5.131030924509056</v>
       </c>
       <c r="G56" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H56" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I56" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>201</v>
+        <v>104</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2190,30 +2190,30 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>11.88448112336965</v>
+        <v>27.807689583568</v>
       </c>
       <c r="D57" t="n">
-        <v>11.64938737985823</v>
+        <v>28.30532509209961</v>
       </c>
       <c r="E57" t="n">
-        <v>20.52815661706435</v>
+        <v>38.9131110442069</v>
       </c>
       <c r="F57" t="n">
-        <v>22.0571469204103</v>
+        <v>38.39640799178323</v>
       </c>
       <c r="G57" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H57" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I57" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>352</v>
+        <v>267</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2221,30 +2221,30 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>4.22716658690096</v>
+        <v>6.494424570845251</v>
       </c>
       <c r="D58" t="n">
-        <v>4.078062042201946</v>
+        <v>6.561999198785587</v>
       </c>
       <c r="E58" t="n">
-        <v>7.895614659313285</v>
+        <v>12.40999940954175</v>
       </c>
       <c r="F58" t="n">
-        <v>7.953327437960121</v>
+        <v>13.08518697200877</v>
       </c>
       <c r="G58" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H58" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I58" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2252,30 +2252,30 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>25.7047945205479</v>
+        <v>31.08532366371205</v>
       </c>
       <c r="D59" t="n">
-        <v>26.4080654752112</v>
+        <v>28.75255634326168</v>
       </c>
       <c r="E59" t="n">
-        <v>44.51105846808795</v>
+        <v>46.6180234833659</v>
       </c>
       <c r="F59" t="n">
-        <v>44.19823482242784</v>
+        <v>46.44136761137902</v>
       </c>
       <c r="G59" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H59" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I59" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2283,30 +2283,30 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>20.7621526418786</v>
+        <v>10.7231370351233</v>
       </c>
       <c r="D60" t="n">
-        <v>20.74461356507922</v>
+        <v>11.67267434047603</v>
       </c>
       <c r="E60" t="n">
-        <v>31.05842752468935</v>
+        <v>21.1406113768457</v>
       </c>
       <c r="F60" t="n">
-        <v>31.86879059261366</v>
+        <v>21.690471736762</v>
       </c>
       <c r="G60" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H60" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I60" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>377</v>
+        <v>201</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -2314,30 +2314,30 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>3.937582080340145</v>
+        <v>11.88448112336965</v>
       </c>
       <c r="D61" t="n">
-        <v>4.077608010263436</v>
+        <v>11.60809420697896</v>
       </c>
       <c r="E61" t="n">
-        <v>8.131539064673124</v>
+        <v>20.52815661706435</v>
       </c>
       <c r="F61" t="n">
-        <v>8.016913327125826</v>
+        <v>21.89146811482703</v>
       </c>
       <c r="G61" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H61" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I61" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -2345,30 +2345,30 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>27.94282171025315</v>
+        <v>25.35435865504355</v>
       </c>
       <c r="D62" t="n">
-        <v>27.09738565871412</v>
+        <v>27.11562952876371</v>
       </c>
       <c r="E62" t="n">
-        <v>36.58958904109585</v>
+        <v>44.7239025529265</v>
       </c>
       <c r="F62" t="n">
-        <v>37.503695855593</v>
+        <v>45.47018386346709</v>
       </c>
       <c r="G62" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H62" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I62" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>227</v>
+        <v>36</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2376,30 +2376,30 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>12.07970116932575</v>
+        <v>27.47558094392985</v>
       </c>
       <c r="D63" t="n">
-        <v>11.6935256612414</v>
+        <v>26.83826510683518</v>
       </c>
       <c r="E63" t="n">
-        <v>21.9335213537469</v>
+        <v>44.52561048243</v>
       </c>
       <c r="F63" t="n">
-        <v>21.70960019178301</v>
+        <v>45.16496584328655</v>
       </c>
       <c r="G63" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H63" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I63" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>445</v>
+        <v>287</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2407,30 +2407,30 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.998666764339605</v>
+        <v>6.50153928163338</v>
       </c>
       <c r="D64" t="n">
-        <v>2.851278003457044</v>
+        <v>6.57848918944739</v>
       </c>
       <c r="E64" t="n">
-        <v>5.148508446205935</v>
+        <v>13.16808822262425</v>
       </c>
       <c r="F64" t="n">
-        <v>5.224618266226475</v>
+        <v>13.06550126729162</v>
       </c>
       <c r="G64" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H64" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I64" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2438,30 +2438,30 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>28.70471824229745</v>
+        <v>29.07700898882855</v>
       </c>
       <c r="D65" t="n">
-        <v>28.22458591806759</v>
+        <v>28.83900787670545</v>
       </c>
       <c r="E65" t="n">
-        <v>40.8530402320128</v>
+        <v>39.83680291200081</v>
       </c>
       <c r="F65" t="n">
-        <v>38.31760586229031</v>
+        <v>39.59914515877343</v>
       </c>
       <c r="G65" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H65" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I65" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>137</v>
+        <v>357</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2469,30 +2469,30 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>20.66005377561415</v>
+        <v>4.03124483715226</v>
       </c>
       <c r="D66" t="n">
-        <v>20.70465284618295</v>
+        <v>4.092111361511472</v>
       </c>
       <c r="E66" t="n">
-        <v>31.62597394361085</v>
+        <v>7.79105743991469</v>
       </c>
       <c r="F66" t="n">
-        <v>31.63900394542166</v>
+        <v>7.965341625519886</v>
       </c>
       <c r="G66" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H66" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I66" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>404</v>
+        <v>13</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2500,30 +2500,30 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.943716322722215</v>
+        <v>30.2600856164383</v>
       </c>
       <c r="D67" t="n">
-        <v>2.856919432982891</v>
+        <v>27.37569926646972</v>
       </c>
       <c r="E67" t="n">
-        <v>5.139842183967665</v>
+        <v>49.0647945205479</v>
       </c>
       <c r="F67" t="n">
-        <v>5.195775405231555</v>
+        <v>45.70233924239862</v>
       </c>
       <c r="G67" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H67" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I67" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2531,30 +2531,30 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>11.539167284601</v>
+        <v>11.5916934479572</v>
       </c>
       <c r="D68" t="n">
-        <v>11.61981931702945</v>
+        <v>11.68939143835429</v>
       </c>
       <c r="E68" t="n">
-        <v>21.5233070866141</v>
+        <v>21.57208323108675</v>
       </c>
       <c r="F68" t="n">
-        <v>22.07364878337297</v>
+        <v>21.72823520947137</v>
       </c>
       <c r="G68" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H68" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I68" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -2562,30 +2562,30 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>6.482027859083125</v>
+        <v>6.369009863195664</v>
       </c>
       <c r="D69" t="n">
-        <v>6.498170648054908</v>
+        <v>6.564271066737621</v>
       </c>
       <c r="E69" t="n">
-        <v>12.0709314117598</v>
+        <v>14.39433555216485</v>
       </c>
       <c r="F69" t="n">
-        <v>13.36141384907853</v>
+        <v>13.08988394036808</v>
       </c>
       <c r="G69" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H69" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I69" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>48</v>
+        <v>315</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -2593,30 +2593,30 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>27.2432984152565</v>
+        <v>6.463069103550845</v>
       </c>
       <c r="D70" t="n">
-        <v>26.41209859625933</v>
+        <v>6.569382265293495</v>
       </c>
       <c r="E70" t="n">
-        <v>43.96776511160066</v>
+        <v>13.4357117067585</v>
       </c>
       <c r="F70" t="n">
-        <v>44.43479437907087</v>
+        <v>13.36752069208861</v>
       </c>
       <c r="G70" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H70" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I70" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>382</v>
+        <v>307</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -2624,30 +2624,30 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>4.215885513358515</v>
+        <v>6.4811635981898</v>
       </c>
       <c r="D71" t="n">
-        <v>4.083765065237531</v>
+        <v>6.54071380721776</v>
       </c>
       <c r="E71" t="n">
-        <v>8.387584415584413</v>
+        <v>13.163863100805</v>
       </c>
       <c r="F71" t="n">
-        <v>8.00207930499567</v>
+        <v>13.3142600552903</v>
       </c>
       <c r="G71" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H71" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I71" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>297</v>
+        <v>266</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2655,30 +2655,30 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>6.465400176089595</v>
+        <v>6.674510079875365</v>
       </c>
       <c r="D72" t="n">
-        <v>6.516478598706382</v>
+        <v>6.571214675129896</v>
       </c>
       <c r="E72" t="n">
-        <v>12.8205039608584</v>
+        <v>13.559449500557</v>
       </c>
       <c r="F72" t="n">
-        <v>13.38441593678373</v>
+        <v>13.07058866814669</v>
       </c>
       <c r="G72" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H72" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I72" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>249</v>
+        <v>67</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2686,30 +2686,30 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>11.35561806914545</v>
+        <v>28.98839950468225</v>
       </c>
       <c r="D73" t="n">
-        <v>11.75876244130113</v>
+        <v>28.854278086145</v>
       </c>
       <c r="E73" t="n">
-        <v>22.42221936195635</v>
+        <v>40.3817006978547</v>
       </c>
       <c r="F73" t="n">
-        <v>22.16576568452618</v>
+        <v>39.63292228328791</v>
       </c>
       <c r="G73" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H73" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I73" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>47</v>
+        <v>175</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2717,30 +2717,30 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>27.59414003044135</v>
+        <v>20.57662109394945</v>
       </c>
       <c r="D74" t="n">
-        <v>26.2999966996789</v>
+        <v>20.49298139488938</v>
       </c>
       <c r="E74" t="n">
-        <v>45.24801162308005</v>
+        <v>31.6523102099372</v>
       </c>
       <c r="F74" t="n">
-        <v>44.56123297347213</v>
+        <v>31.0143681931411</v>
       </c>
       <c r="G74" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H74" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I74" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>320</v>
+        <v>183</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2748,30 +2748,30 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>6.737143782051575</v>
+        <v>20.50486564243355</v>
       </c>
       <c r="D75" t="n">
-        <v>6.516553274868645</v>
+        <v>20.90406351724012</v>
       </c>
       <c r="E75" t="n">
-        <v>12.7590167072393</v>
+        <v>30.93111418799845</v>
       </c>
       <c r="F75" t="n">
-        <v>12.77600587003324</v>
+        <v>31.11085343214394</v>
       </c>
       <c r="G75" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H75" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I75" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2779,30 +2779,30 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>27.2872921397699</v>
+        <v>27.1198465489989</v>
       </c>
       <c r="D76" t="n">
-        <v>26.99616229663116</v>
+        <v>27.42976482309763</v>
       </c>
       <c r="E76" t="n">
-        <v>36.72890203403895</v>
+        <v>38.83181914262525</v>
       </c>
       <c r="F76" t="n">
-        <v>37.43940312920161</v>
+        <v>37.27087117449805</v>
       </c>
       <c r="G76" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H76" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I76" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>79</v>
+        <v>165</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2810,30 +2810,30 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>28.7826548331082</v>
+        <v>20.46775029616</v>
       </c>
       <c r="D77" t="n">
-        <v>28.68301980391864</v>
+        <v>20.8072154841959</v>
       </c>
       <c r="E77" t="n">
-        <v>39.984582783416</v>
+        <v>31.0622193139191</v>
       </c>
       <c r="F77" t="n">
-        <v>38.90181774854081</v>
+        <v>31.18391604479205</v>
       </c>
       <c r="G77" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H77" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I77" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>136</v>
+        <v>365</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -2841,30 +2841,30 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>21.0279808954466</v>
+        <v>4.155383745283665</v>
       </c>
       <c r="D78" t="n">
-        <v>20.58313072312434</v>
+        <v>4.096930448643548</v>
       </c>
       <c r="E78" t="n">
-        <v>31.15803633286095</v>
+        <v>8.333400832356144</v>
       </c>
       <c r="F78" t="n">
-        <v>31.55074876936997</v>
+        <v>7.975099802787324</v>
       </c>
       <c r="G78" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H78" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I78" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>459</v>
+        <v>353</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -2872,30 +2872,30 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>3.040076674111135</v>
+        <v>4.046439073370145</v>
       </c>
       <c r="D79" t="n">
-        <v>2.859152550770598</v>
+        <v>4.095099111817168</v>
       </c>
       <c r="E79" t="n">
-        <v>5.42513506589483</v>
+        <v>8.20925790237513</v>
       </c>
       <c r="F79" t="n">
-        <v>5.235857041043209</v>
+        <v>7.956990423803667</v>
       </c>
       <c r="G79" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H79" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I79" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>256</v>
+        <v>160</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -2903,30 +2903,30 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>11.66866226575255</v>
+        <v>21.47186366087795</v>
       </c>
       <c r="D80" t="n">
-        <v>11.57123381288641</v>
+        <v>20.85259524482403</v>
       </c>
       <c r="E80" t="n">
-        <v>20.67602344286265</v>
+        <v>31.07686480805305</v>
       </c>
       <c r="F80" t="n">
-        <v>21.567395438499</v>
+        <v>31.26086725188187</v>
       </c>
       <c r="G80" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H80" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I80" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>63</v>
+        <v>422</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -2934,30 +2934,30 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>25.34126856221935</v>
+        <v>2.857982388115895</v>
       </c>
       <c r="D81" t="n">
-        <v>26.47280752843108</v>
+        <v>2.876360596186229</v>
       </c>
       <c r="E81" t="n">
-        <v>41.2648858447488</v>
+        <v>5.15475650441901</v>
       </c>
       <c r="F81" t="n">
-        <v>44.20598408652414</v>
+        <v>5.222528391717137</v>
       </c>
       <c r="G81" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H81" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I81" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>283</v>
+        <v>341</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2965,30 +2965,30 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>6.507980967283135</v>
+        <v>4.30861957506476</v>
       </c>
       <c r="D82" t="n">
-        <v>6.538690287479841</v>
+        <v>4.091311711192263</v>
       </c>
       <c r="E82" t="n">
-        <v>12.67362242715445</v>
+        <v>7.80812461680692</v>
       </c>
       <c r="F82" t="n">
-        <v>13.14429346367833</v>
+        <v>7.951013236744478</v>
       </c>
       <c r="G82" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H82" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I82" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>337</v>
+        <v>260</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -2996,30 +2996,30 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4.039254631720381</v>
+        <v>12.05705788821515</v>
       </c>
       <c r="D83" t="n">
-        <v>4.080867635912815</v>
+        <v>11.77742091375441</v>
       </c>
       <c r="E83" t="n">
-        <v>8.12406385658301</v>
+        <v>20.6809939223637</v>
       </c>
       <c r="F83" t="n">
-        <v>7.975573573066458</v>
+        <v>22.11841761831622</v>
       </c>
       <c r="G83" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H83" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I83" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -3027,30 +3027,30 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>11.6451410367553</v>
+        <v>11.46401006916955</v>
       </c>
       <c r="D84" t="n">
-        <v>11.7137124150639</v>
+        <v>11.62883944202712</v>
       </c>
       <c r="E84" t="n">
-        <v>21.72440284332905</v>
+        <v>22.12986626121865</v>
       </c>
       <c r="F84" t="n">
-        <v>21.88753926728712</v>
+        <v>21.6825460433715</v>
       </c>
       <c r="G84" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H84" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I84" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>251</v>
+        <v>290</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -3058,30 +3058,30 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>11.4244775841461</v>
+        <v>6.432269068475815</v>
       </c>
       <c r="D85" t="n">
-        <v>11.7438862009162</v>
+        <v>6.559608248615911</v>
       </c>
       <c r="E85" t="n">
-        <v>22.13426179604255</v>
+        <v>13.13820623352755</v>
       </c>
       <c r="F85" t="n">
-        <v>22.17295303021226</v>
+        <v>13.05934661068983</v>
       </c>
       <c r="G85" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H85" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I85" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -3089,30 +3089,30 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>27.62308252266555</v>
+        <v>19.6720855401965</v>
       </c>
       <c r="D86" t="n">
-        <v>27.17122118772152</v>
+        <v>20.8871878261552</v>
       </c>
       <c r="E86" t="n">
-        <v>44.3145383604054</v>
+        <v>31.1440779547959</v>
       </c>
       <c r="F86" t="n">
-        <v>44.49598626478281</v>
+        <v>31.24608064620595</v>
       </c>
       <c r="G86" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H86" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I86" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>7</v>
+        <v>305</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -3120,30 +3120,30 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>29.22831050228305</v>
+        <v>6.534782916012954</v>
       </c>
       <c r="D87" t="n">
-        <v>28.28390075232117</v>
+        <v>6.548428311074352</v>
       </c>
       <c r="E87" t="n">
-        <v>48.07222222222215</v>
+        <v>13.12253347698935</v>
       </c>
       <c r="F87" t="n">
-        <v>46.27206132850507</v>
+        <v>13.2840934346164</v>
       </c>
       <c r="G87" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H87" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I87" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>279</v>
+        <v>346</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -3151,30 +3151,30 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>6.275282812211669</v>
+        <v>3.938476884053975</v>
       </c>
       <c r="D88" t="n">
-        <v>6.525791884668312</v>
+        <v>4.08904716554579</v>
       </c>
       <c r="E88" t="n">
-        <v>13.6903039898968</v>
+        <v>7.439953571899714</v>
       </c>
       <c r="F88" t="n">
-        <v>13.09721309104078</v>
+        <v>7.974953555003599</v>
       </c>
       <c r="G88" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H88" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I88" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>91</v>
+        <v>461</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -3182,30 +3182,30 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>27.7032903257572</v>
+        <v>2.85074914383561</v>
       </c>
       <c r="D89" t="n">
-        <v>28.57010582518382</v>
+        <v>2.876072398038026</v>
       </c>
       <c r="E89" t="n">
-        <v>38.10147801009365</v>
+        <v>5.361368397674685</v>
       </c>
       <c r="F89" t="n">
-        <v>38.72797098314681</v>
+        <v>5.184774884850547</v>
       </c>
       <c r="G89" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H89" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I89" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>452</v>
+        <v>128</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -3213,30 +3213,30 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2.996457392159715</v>
+        <v>27.94282171025315</v>
       </c>
       <c r="D90" t="n">
-        <v>2.849413370157303</v>
+        <v>27.41413823856061</v>
       </c>
       <c r="E90" t="n">
-        <v>4.96057993703735</v>
+        <v>36.58958904109585</v>
       </c>
       <c r="F90" t="n">
-        <v>5.242253618250685</v>
+        <v>37.3094995478669</v>
       </c>
       <c r="G90" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H90" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I90" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>197</v>
+        <v>268</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -3244,30 +3244,30 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>20.0223325313824</v>
+        <v>6.57464282390954</v>
       </c>
       <c r="D91" t="n">
-        <v>20.76794587615861</v>
+        <v>6.553012557480769</v>
       </c>
       <c r="E91" t="n">
-        <v>31.1599641950344</v>
+        <v>11.98946943738485</v>
       </c>
       <c r="F91" t="n">
-        <v>30.44883266330862</v>
+        <v>13.09570386460891</v>
       </c>
       <c r="G91" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H91" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I91" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>5</v>
+        <v>355</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -3275,30 +3275,30 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>28.00781348788195</v>
+        <v>3.96170938594873</v>
       </c>
       <c r="D92" t="n">
-        <v>28.16831739109713</v>
+        <v>4.090104975597078</v>
       </c>
       <c r="E92" t="n">
-        <v>45.87929984779295</v>
+        <v>7.833063172243235</v>
       </c>
       <c r="F92" t="n">
-        <v>46.29575479277739</v>
+        <v>7.975478550183213</v>
       </c>
       <c r="G92" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H92" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I92" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -3306,30 +3306,30 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>27.36924867030145</v>
+        <v>25.34126856221935</v>
       </c>
       <c r="D93" t="n">
-        <v>28.09151798302076</v>
+        <v>26.32659561312587</v>
       </c>
       <c r="E93" t="n">
-        <v>38.34450661918775</v>
+        <v>41.2648858447488</v>
       </c>
       <c r="F93" t="n">
-        <v>38.20215239448641</v>
+        <v>43.95413671378734</v>
       </c>
       <c r="G93" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H93" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I93" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -3337,25 +3337,25 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>20.88558337703505</v>
+        <v>27.44204718417045</v>
       </c>
       <c r="D94" t="n">
-        <v>20.76519244426394</v>
+        <v>26.35923708197695</v>
       </c>
       <c r="E94" t="n">
-        <v>30.6067392859107</v>
+        <v>43.2413534714904</v>
       </c>
       <c r="F94" t="n">
-        <v>31.23280544717642</v>
+        <v>44.06749481393824</v>
       </c>
       <c r="G94" t="n">
-        <v>0.4416636445390975</v>
+        <v>0.5778243081676049</v>
       </c>
       <c r="H94" t="n">
-        <v>0.664577794196509</v>
+        <v>0.7601475568385423</v>
       </c>
       <c r="I94" t="n">
-        <v>0.9966857799672354</v>
+        <v>0.9952405461750589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>